<commit_message>
Fixed the download report api bug and saving file in tmp folder
</commit_message>
<xml_diff>
--- a/reports/report.export.xlsx
+++ b/reports/report.export.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,9 +419,757 @@
         <v>points</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v xml:space="preserve">Rupapara Princy Hareshkumar </v>
+      </c>
+      <c r="B2">
+        <v>20221203001</v>
+      </c>
+      <c r="C2" t="str">
+        <v>princyrupapara18@gmail.com</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Chettiyar Prashant</v>
+      </c>
+      <c r="B3">
+        <v>20221203002</v>
+      </c>
+      <c r="C3" t="str">
+        <v>prashantchettiyar@ieee.org</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Parth Patel</v>
+      </c>
+      <c r="B4">
+        <v>20221203003</v>
+      </c>
+      <c r="C4" t="str">
+        <v>ppatel7802@gmail.com</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">Bairwa Ishita mahendrabhai </v>
+      </c>
+      <c r="B5">
+        <v>20221203005</v>
+      </c>
+      <c r="C5" t="str">
+        <v>player58558@gmail.com</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Lay maheshbhai thakkar</v>
+      </c>
+      <c r="B6">
+        <v>20221203007</v>
+      </c>
+      <c r="C6" t="str">
+        <v>layyyythakkar@gmail.com</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Shah Rakesh Jagdishchandra</v>
+      </c>
+      <c r="B7">
+        <v>20221203006</v>
+      </c>
+      <c r="C7" t="str">
+        <v>rakeshshah.ce@socet.edu.in</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>RUSHI HITESH PRAJAPATI</v>
+      </c>
+      <c r="B8">
+        <v>20221203004</v>
+      </c>
+      <c r="C8" t="str">
+        <v>prajapatirushih@gmail.com</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Jil Upadhyay</v>
+      </c>
+      <c r="B9">
+        <v>20221203015</v>
+      </c>
+      <c r="C9" t="str">
+        <v>upadhyay.jil1802@gmail.com</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Govind Godara</v>
+      </c>
+      <c r="B10">
+        <v>20221203012</v>
+      </c>
+      <c r="C10" t="str">
+        <v>godaragovind02@gmail.com</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">Danish salmani </v>
+      </c>
+      <c r="B11">
+        <v>20221203016</v>
+      </c>
+      <c r="C11" t="str">
+        <v>danishsalmani9010@gmail.com</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">Dev Shinde </v>
+      </c>
+      <c r="B12">
+        <v>20221203014</v>
+      </c>
+      <c r="C12" t="str">
+        <v>200103062031@silveroakuni.ac.in</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Viraj Modi</v>
+      </c>
+      <c r="B13">
+        <v>20221203011</v>
+      </c>
+      <c r="C13" t="str">
+        <v>virajmodi43@gmail.com</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Gautam Premjee Bhanushali</v>
+      </c>
+      <c r="B14">
+        <v>20221203010</v>
+      </c>
+      <c r="C14" t="str">
+        <v>bhanushaligautam6355@gmail.com</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">Aryan Acharya </v>
+      </c>
+      <c r="B15">
+        <v>20221203013</v>
+      </c>
+      <c r="C15" t="str">
+        <v>aryanacharya12003@gmail.com</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v xml:space="preserve">Dev Shinde </v>
+      </c>
+      <c r="B16">
+        <v>20221203018</v>
+      </c>
+      <c r="C16" t="str">
+        <v>shindedev123@gmail.com</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Jenish soni</v>
+      </c>
+      <c r="B17">
+        <v>20221203017</v>
+      </c>
+      <c r="C17" t="str">
+        <v>sonijenish290804@gmail.com</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Jaimin Somaiya</v>
+      </c>
+      <c r="B18">
+        <v>20221203021</v>
+      </c>
+      <c r="C18" t="str">
+        <v>190770107277@socet.edu.in</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Kavish Shah</v>
+      </c>
+      <c r="B19">
+        <v>20221203019</v>
+      </c>
+      <c r="C19" t="str">
+        <v>kavishmshah2004@gmail.com</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v xml:space="preserve">Sama Mohd Mustufa </v>
+      </c>
+      <c r="B20">
+        <v>20221203020</v>
+      </c>
+      <c r="C20" t="str">
+        <v>samamustufa9824@gmail.com</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Patel dhruvbhai</v>
+      </c>
+      <c r="B21">
+        <v>20221203022</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Pateldhruv7067733@gmail.com</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Divy shah</v>
+      </c>
+      <c r="B22">
+        <v>20221203023</v>
+      </c>
+      <c r="C22" t="str">
+        <v>shahdivy031@gmail.com</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve">Poojan Jain </v>
+      </c>
+      <c r="B23">
+        <v>20221203024</v>
+      </c>
+      <c r="C23" t="str">
+        <v>200103052010@silveroakuni.ac.in</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v xml:space="preserve">Yash G. Mangnani </v>
+      </c>
+      <c r="B24">
+        <v>20221203025</v>
+      </c>
+      <c r="C24" t="str">
+        <v>yashmangnani@gmail.com</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v xml:space="preserve">PREET SINGHA </v>
+      </c>
+      <c r="B25">
+        <v>20221203008</v>
+      </c>
+      <c r="C25" t="str">
+        <v>preetsingha141@gmail.com</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Yash Bhatt</v>
+      </c>
+      <c r="B26">
+        <v>20221203028</v>
+      </c>
+      <c r="C26" t="str">
+        <v>yabh678@gmail.com</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Sunil Parmar </v>
+      </c>
+      <c r="B27">
+        <v>20221203029</v>
+      </c>
+      <c r="C27" t="str">
+        <v>shp00027@gmail.com</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Prasad Tejus Raghavendra</v>
+      </c>
+      <c r="B28">
+        <v>20221203030</v>
+      </c>
+      <c r="C28" t="str">
+        <v>tejusraghavendra09@gmail.com</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v xml:space="preserve">Harsh solanki </v>
+      </c>
+      <c r="B29">
+        <v>20221203031</v>
+      </c>
+      <c r="C29" t="str">
+        <v>harshsolanki0212@gmail.com</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Vachhani manthan Dipakbhai</v>
+      </c>
+      <c r="B30">
+        <v>20221203032</v>
+      </c>
+      <c r="C30" t="str">
+        <v>vacmanthan@gmail.com</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Divyesh Patel</v>
+      </c>
+      <c r="B31">
+        <v>20221203009</v>
+      </c>
+      <c r="C31" t="str">
+        <v>pateldivyesh2309@gmail.com</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v xml:space="preserve">Pipaliya Arjun </v>
+      </c>
+      <c r="B32">
+        <v>20221203034</v>
+      </c>
+      <c r="C32" t="str">
+        <v>arjunpipaliya2005@gmail.com</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v xml:space="preserve">Abhay Pisharodi </v>
+      </c>
+      <c r="B33">
+        <v>20221203027</v>
+      </c>
+      <c r="C33" t="str">
+        <v>abhayvg.2904@gmail.com</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>parth panchal manojkumar</v>
+      </c>
+      <c r="B34">
+        <v>20221203035</v>
+      </c>
+      <c r="C34" t="str">
+        <v>210133062006@silvroakuni.ac.in</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Alok rathor</v>
+      </c>
+      <c r="B35">
+        <v>20221203036</v>
+      </c>
+      <c r="C35" t="str">
+        <v>alokrathore082@gmail.com</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v xml:space="preserve">Lalit Suthar </v>
+      </c>
+      <c r="B36">
+        <v>20221203037</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Lalitsutharclg@gmail.com</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Hiren Dineshbhai Parmar</v>
+      </c>
+      <c r="B37">
+        <v>20221203038</v>
+      </c>
+      <c r="C37" t="str">
+        <v>hiren33433@gmail.com</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Himanshu Jogi</v>
+      </c>
+      <c r="B38">
+        <v>20221203039</v>
+      </c>
+      <c r="C38" t="str">
+        <v>200103072030@silveroakuni.ac.in</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Kinjal Rameshchandra Sumera</v>
+      </c>
+      <c r="B39">
+        <v>20221203040</v>
+      </c>
+      <c r="C39" t="str">
+        <v>kinjalsumera53@gmail.com</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v xml:space="preserve">Hotri Trivedi </v>
+      </c>
+      <c r="B40">
+        <v>20221203041</v>
+      </c>
+      <c r="C40" t="str">
+        <v>trivedihh2@gmail.com</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v xml:space="preserve">kathan Mistry </v>
+      </c>
+      <c r="B41">
+        <v>20221203044</v>
+      </c>
+      <c r="C41" t="str">
+        <v>kathanmistry2004@gmail.com</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Hardik H Soni</v>
+      </c>
+      <c r="B42">
+        <v>20221203042</v>
+      </c>
+      <c r="C42" t="str">
+        <v>hardiksoni7203@gmail.com</v>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Gautam Patidar</v>
+      </c>
+      <c r="B43">
+        <v>20221203043</v>
+      </c>
+      <c r="C43" t="str">
+        <v>200103072051@silveroakuni.ac.in</v>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v xml:space="preserve">Darshan Dilipbhai Satapara </v>
+      </c>
+      <c r="B44">
+        <v>20221203026</v>
+      </c>
+      <c r="C44" t="str">
+        <v>darshansatapara286@gmail.com</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>MEET PATEL</v>
+      </c>
+      <c r="B45">
+        <v>20221203033</v>
+      </c>
+      <c r="C45" t="str">
+        <v>pmk31124@gmail.com</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E45"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>